<commit_message>
Feat: Add all advanced tracking features - Email, Eftikad, Liturgy, Excel Export, Announcements
</commit_message>
<xml_diff>
--- a/export_attendance_data.xlsx
+++ b/export_attendance_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L150"/>
+  <dimension ref="A1:L151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7829,6 +7829,48 @@
         </is>
       </c>
       <c r="L150" t="inlineStr"/>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>150</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fady </t>
+        </is>
+      </c>
+      <c r="C151" t="n">
+        <v>8</v>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Massoud</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>213456yu</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>231423546</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="I151" t="inlineStr"/>
+      <c r="J151" t="inlineStr"/>
+      <c r="K151" t="inlineStr"/>
+      <c r="L151" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7841,7 +7883,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7869,12 +7911,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Bishoy Arsalyos</t>
+          <t>Christin Wasef</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -7886,12 +7928,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Cristiano Gerges (Attia?)</t>
+          <t>Jonathan Seif</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -7903,17 +7945,629 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Mira Malty</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2026-01-31</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Novear Mikhael </t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2026-01-31</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Philopateer Kaldas</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2026-01-31</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Salah Salib</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2026-01-31</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Shady Aziz</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2026-01-31</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Shenouda Hanna</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2026-01-31</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Shenouda Saeed</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2026-01-31</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Thomas Keliny</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2026-01-31</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Thomas Masoued</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2026-01-31</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Torres Ibrahim </t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2026-01-31</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Wanas Youns/Abdelshahid</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2026-01-31</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Yustos Bostros</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2026-01-31</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Bishoy Arsalyos</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Cristiano Gerges (Attia?)</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
           <t>Danny Soliman</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B18" t="inlineStr">
         <is>
           <t>2026-01-25</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>present</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Fady Reda</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Georgino Bebawy</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Ishak Kamel</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>John Yehia</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jotham Shenouda </t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Joyce Zaki</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Justin Fakoury</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Karas Eshak Abdelmalak</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Karas Fares</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Karas Monir</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Karas Moura</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Karas Shehata </t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Kyrollos Soliman</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Madonna Girgis</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Maria Attiya</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Mariam Ibrahim</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Marly Abdelshehed</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Marseleno Mina</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Monica Ramsis</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sabrina Kamel </t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Sandy Ibrahim</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Verena Abdelmalak</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>absent</t>
         </is>
       </c>
     </row>

</xml_diff>